<commit_message>
Anpassung Sheetname (Reiter), datentypen spalten korrigiert
</commit_message>
<xml_diff>
--- a/src/Nummerneinteilung.xlsx
+++ b/src/Nummerneinteilung.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CH00BZS\git\Nummerneinteilung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CH00BZS\git\Nummerneinteilung\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C9EA744-1478-4D92-9193-A5C66E1F169B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E4C2203-BAA0-48B4-BEF5-B9D5AD754ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -355,7 +354,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,36 +376,36 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>44622</v>
-      </c>
-      <c r="B2" s="1">
-        <v>44625</v>
-      </c>
-      <c r="C2" s="1">
-        <v>44622</v>
+      <c r="A2">
+        <v>20220302</v>
+      </c>
+      <c r="B2">
+        <v>20220305</v>
+      </c>
+      <c r="C2">
+        <v>20220302</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>44635</v>
-      </c>
-      <c r="B3" s="1">
-        <v>44635</v>
-      </c>
-      <c r="C3" s="1">
-        <v>44632</v>
+      <c r="A3">
+        <v>20220315</v>
+      </c>
+      <c r="B3">
+        <v>20220315</v>
+      </c>
+      <c r="C3">
+        <v>20220312</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>44646</v>
-      </c>
-      <c r="B4" s="1">
-        <v>44644</v>
-      </c>
-      <c r="C4" s="1">
-        <v>44646</v>
+      <c r="A4">
+        <v>20220326</v>
+      </c>
+      <c r="B4">
+        <v>20220324</v>
+      </c>
+      <c r="C4">
+        <v>20220326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel erweitert, import angepasst
</commit_message>
<xml_diff>
--- a/src/Nummerneinteilung.xlsx
+++ b/src/Nummerneinteilung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CH00BZS\git\Nummerneinteilung\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E4C2203-BAA0-48B4-BEF5-B9D5AD754ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5FA29B-1AA5-4DD5-8846-03A01FCA6728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>nummer1</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>nummer3</t>
+  </si>
+  <si>
+    <t>nummer4</t>
+  </si>
+  <si>
+    <t>nummer5</t>
   </si>
 </sst>
 </file>
@@ -351,20 +357,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="3" max="5" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -374,8 +380,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20220302</v>
       </c>
@@ -385,8 +397,14 @@
       <c r="C2">
         <v>20220302</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>20220305</v>
+      </c>
+      <c r="E2">
+        <v>20220302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20220315</v>
       </c>
@@ -396,8 +414,14 @@
       <c r="C3">
         <v>20220312</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>20220332</v>
+      </c>
+      <c r="E3">
+        <v>20220312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20220326</v>
       </c>
@@ -406,6 +430,46 @@
       </c>
       <c r="C4">
         <v>20220326</v>
+      </c>
+      <c r="D4">
+        <v>20220324</v>
+      </c>
+      <c r="E4">
+        <v>20220326</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>20220405</v>
+      </c>
+      <c r="B5">
+        <v>20220408</v>
+      </c>
+      <c r="C5">
+        <v>20220405</v>
+      </c>
+      <c r="D5">
+        <v>20220405</v>
+      </c>
+      <c r="E5">
+        <v>20220401</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>20220501</v>
+      </c>
+      <c r="B6">
+        <v>20220507</v>
+      </c>
+      <c r="C6">
+        <v>20220509</v>
+      </c>
+      <c r="D6">
+        <v>20220501</v>
+      </c>
+      <c r="E6">
+        <v>20220501</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ausbau um die top 3 übereinstimmenden Werte auszugeben
</commit_message>
<xml_diff>
--- a/src/Nummerneinteilung.xlsx
+++ b/src/Nummerneinteilung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CH00BZS\git\Nummerneinteilung\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5FA29B-1AA5-4DD5-8846-03A01FCA6728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75440363-4E36-4D19-997A-8655CE576CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>nummer1</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>nummer5</t>
+  </si>
+  <si>
+    <t>nummer6</t>
   </si>
 </sst>
 </file>
@@ -357,20 +360,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="5" width="19.42578125" customWidth="1"/>
+    <col min="3" max="6" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -386,8 +389,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20220302</v>
       </c>
@@ -403,8 +409,11 @@
       <c r="E2">
         <v>20220302</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>20220301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20220315</v>
       </c>
@@ -420,8 +429,11 @@
       <c r="E3">
         <v>20220312</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>20220312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20220326</v>
       </c>
@@ -437,8 +449,11 @@
       <c r="E4">
         <v>20220326</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>20220325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20220405</v>
       </c>
@@ -454,8 +469,11 @@
       <c r="E5">
         <v>20220401</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>20220401</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20220501</v>
       </c>
@@ -470,6 +488,29 @@
       </c>
       <c r="E6">
         <v>20220501</v>
+      </c>
+      <c r="F6">
+        <v>20220501</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>20220601</v>
+      </c>
+      <c r="B7">
+        <v>20220602</v>
+      </c>
+      <c r="C7">
+        <v>20220601</v>
+      </c>
+      <c r="D7">
+        <v>20220604</v>
+      </c>
+      <c r="E7">
+        <v>20220605</v>
+      </c>
+      <c r="F7">
+        <v>20220605</v>
       </c>
     </row>
   </sheetData>

</xml_diff>